<commit_message>
Finally finished the killme graph
</commit_message>
<xml_diff>
--- a/TAKEHOMEFINAL/WorkSheet.xlsx
+++ b/TAKEHOMEFINAL/WorkSheet.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gotmi\Documents\GitHub\GrandAnseBeach_SWMM\TAKEHOMEFINAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msc94\Documents\GitHub\GrandAnseBeach_SWMM\TAKEHOMEFINAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABA5319-299A-48AF-84BD-E3D30DB3A2CA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1935" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{46ACFC8D-6A43-42E6-BC46-CF5BF3E67875}"/>
+    <workbookView xWindow="28680" yWindow="1935" windowWidth="20730" windowHeight="11160" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -370,10 +369,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -413,9 +412,9 @@
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -437,22 +436,19 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -461,10 +457,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -781,7 +780,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0201309-F474-4CC0-A187-8A77432B5DB4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1179,16 +1178,16 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="E19" s="14" t="s">
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="E19" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
       <c r="I19" t="s">
         <v>36</v>
       </c>
@@ -1272,31 +1271,31 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="16">
+      <c r="B23" s="15">
         <v>89.107666527021365</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="16">
+      <c r="F23" s="15">
         <v>100</v>
       </c>
-      <c r="G23" s="18" t="s">
+      <c r="G23" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="I23" s="15" t="s">
+      <c r="I23" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J23" s="16">
+      <c r="J23" s="15">
         <v>0</v>
       </c>
-      <c r="K23" s="18" t="s">
+      <c r="K23" s="17" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1542,7 +1541,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CC7DC81-4C38-4F99-AB32-1ADE52FD13DF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -1879,7 +1878,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14D43689-3362-43D4-80C9-3845A28F9F48}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
@@ -1895,11 +1894,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1946,11 +1945,11 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1986,24 +1985,24 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="16">
         <v>200</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="16">
         <v>320</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2030,11 +2029,11 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -2114,11 +2113,11 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -2165,21 +2164,21 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
     </row>
     <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B32" s="19">
+      <c r="B32" s="18">
         <f>2*34^(0.5)/12</f>
         <v>0.97182531580755016</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="17" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2251,7 +2250,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C50870C-EF5B-45B7-A162-20BF1C28EA9E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2271,11 +2270,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA300D36-1580-4D84-9B68-9B7402B0F4AA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2288,30 +2287,30 @@
       <c r="A1" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14" t="s">
+      <c r="E1" s="20"/>
+      <c r="F1" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14" t="s">
+      <c r="G1" s="20"/>
+      <c r="H1" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14" t="s">
+      <c r="I1" s="20"/>
+      <c r="J1" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14" t="s">
+      <c r="K1" s="20"/>
+      <c r="L1" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="M1" s="14"/>
+      <c r="M1" s="20"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
@@ -2356,10 +2355,10 @@
       <c r="A3" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>109</v>
       </c>
       <c r="D3">
@@ -2438,10 +2437,10 @@
       <c r="A5" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>109</v>
       </c>
       <c r="D5">
@@ -2518,13 +2517,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="L1:M1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>